<commit_message>
Small refactoring and document update (Build 378)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint21Plan.xlsx
+++ b/doc/Planning/Sprint21Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>سایر امکانات سرویس وب</t>
+  </si>
+  <si>
+    <t>تحلیل نیازمندی ها و طراحی ساختار اطلاعاتی کارتابل</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1107,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F33" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="A2:F33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F34" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="A2:F34"/>
   <tableColumns count="6">
     <tableColumn id="1" name="هدف کاری" dataDxfId="44"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="43"/>
@@ -1438,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,7 +1490,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1499,7 +1502,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1511,7 +1514,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1523,7 +1526,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1551,7 +1554,7 @@
         <v>56</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1563,7 +1566,7 @@
         <v>57</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1575,7 +1578,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1589,7 +1592,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1603,7 +1606,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1617,7 +1620,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1629,7 +1632,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1641,7 +1644,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1653,7 +1656,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1665,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1707,7 +1710,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1731,7 +1734,7 @@
         <v>52</v>
       </c>
       <c r="C22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1763,26 +1766,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="25" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="B26" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1790,28 +1791,30 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1820,7 +1823,7 @@
     <row r="29" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
@@ -1829,12 +1832,10 @@
       <c r="E29" s="5"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>30</v>
-      </c>
+    <row r="30" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -1844,9 +1845,11 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B31" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -1858,7 +1861,7 @@
     <row r="32" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -1867,20 +1870,32 @@
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
     </row>
+    <row r="34" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33 C13:C17 C20:C24 C3:C10 C26:C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C34 C13:C17 C20:C25 C3:C10">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E34">
       <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>